<commit_message>
Note: Module 15 + Tute 1 & 2
</commit_message>
<xml_diff>
--- a/LIRV/Textbook/LI&R Val S1 2020 M14 Exercise 14.11.xlsx
+++ b/LIRV/Textbook/LI&R Val S1 2020 M14 Exercise 14.11.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Course Development\Fellowship\LIaR Modules\LIaR Valuation\2018 Development\Textbook Q and A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VZhu\Documents\GitHub\my_file\LIRV\Textbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E1108C0-A906-486C-BBB4-FFA9D3B232E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6225" xr2:uid="{F908A768-5603-4024-AD98-7D3873D5A27A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -77,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -205,9 +204,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -217,15 +219,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,11 +596,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B08A88D-44CE-44F4-B81F-C43685440FFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J3:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:R17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,54 +610,54 @@
   </cols>
   <sheetData>
     <row r="3" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8" t="s">
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
     </row>
     <row r="5" spans="10:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="J5" s="9"/>
-      <c r="K5" s="9" t="s">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="M5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="10"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9" t="s">
+      <c r="O5" s="5"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="R5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -701,10 +700,11 @@
         <v>12</v>
       </c>
       <c r="Q7" s="1">
-        <f>1.5</f>
+        <f>(M6-N6)+(M8-N8)</f>
         <v>1.5</v>
       </c>
       <c r="R7" s="1">
+        <f>(M6-N6)</f>
         <v>1</v>
       </c>
     </row>
@@ -728,89 +728,89 @@
         <v>5</v>
       </c>
       <c r="Q8" s="1">
-        <f>50-Q7</f>
+        <f>N8+N6-100</f>
         <v>48.5</v>
       </c>
       <c r="R8" s="1">
-        <f>50-R7</f>
+        <f>M8+N6-100</f>
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="6">
         <f>SUM(K6:K8)</f>
         <v>150</v>
       </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11">
+      <c r="L9" s="6"/>
+      <c r="M9" s="6">
         <v>150</v>
       </c>
-      <c r="N9" s="11">
+      <c r="N9" s="6">
         <f>N8+N6</f>
         <v>148.5</v>
       </c>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11">
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6">
         <f>SUM(Q6:Q8)</f>
         <v>150</v>
       </c>
-      <c r="R9" s="11">
+      <c r="R9" s="6">
         <f>SUM(R6:R8)</f>
         <v>150</v>
       </c>
     </row>
     <row r="11" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
     </row>
     <row r="12" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="8" t="s">
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
     </row>
     <row r="13" spans="10:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="J13" s="9"/>
-      <c r="K13" s="9" t="s">
+      <c r="J13" s="4"/>
+      <c r="K13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="L13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N13" s="10" t="s">
+      <c r="N13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O13" s="10"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9" t="s">
+      <c r="O13" s="5"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="R13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -852,9 +852,11 @@
         <v>12</v>
       </c>
       <c r="Q15" s="1">
+        <f>(M14-N14)+(M16-N16)</f>
         <v>3.5</v>
       </c>
       <c r="R15" s="1">
+        <f>(M14-N14)</f>
         <v>1</v>
       </c>
     </row>
@@ -870,6 +872,7 @@
         <v>50</v>
       </c>
       <c r="N16" s="1">
+        <f>M16*0.95</f>
         <v>47.5</v>
       </c>
       <c r="O16" s="1"/>
@@ -881,33 +884,33 @@
         <v>46.5</v>
       </c>
       <c r="R16" s="1">
-        <f>50-R15</f>
+        <f>M16+N14-100</f>
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="6">
         <f>SUM(K14:K16)</f>
         <v>150</v>
       </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11">
+      <c r="L17" s="6"/>
+      <c r="M17" s="6">
         <v>150</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="6">
         <f>N16+N14</f>
         <v>146.5</v>
       </c>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11">
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6">
         <f>SUM(Q14:Q16)</f>
         <v>150</v>
       </c>
-      <c r="R17" s="11">
+      <c r="R17" s="6">
         <f>SUM(R14:R16)</f>
         <v>150</v>
       </c>

</xml_diff>